<commit_message>
adelantada documentación en diseño y manual usuario, exportados algunos diagramas desde workbench
</commit_message>
<xml_diff>
--- a/PA_Proyecto.xlsx
+++ b/PA_Proyecto.xlsx
@@ -1,19 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\CorePHPMVC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22231EE3-AA03-4852-BCB3-200D6170EAF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Casos de Uso" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Requisitos" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Entidades y Atributos" sheetId="3" r:id="rId5"/>
+    <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
+    <sheet name="Requisitos" sheetId="2" r:id="rId2"/>
+    <sheet name="Entidades y Atributos" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabla Crud" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="143">
   <si>
     <t>TODO</t>
   </si>
@@ -114,9 +124,6 @@
     <t>Petición</t>
   </si>
   <si>
-    <t>Notificación(denuncia)</t>
-  </si>
-  <si>
     <t>Comentarios</t>
   </si>
   <si>
@@ -162,9 +169,6 @@
     <t>Provincia</t>
   </si>
   <si>
-    <t>Crear(admin)</t>
-  </si>
-  <si>
     <t>Images</t>
   </si>
   <si>
@@ -174,18 +178,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>Eliminar(marcar)</t>
-  </si>
-  <si>
-    <t>crear</t>
-  </si>
-  <si>
-    <t>crear(include)</t>
-  </si>
-  <si>
-    <t>Crear</t>
-  </si>
-  <si>
     <t>uuid</t>
   </si>
   <si>
@@ -195,36 +187,18 @@
     <t>name</t>
   </si>
   <si>
-    <t>Actualizar(admin)</t>
-  </si>
-  <si>
     <t>user_id</t>
   </si>
   <si>
     <t>ad_id</t>
   </si>
   <si>
-    <t>Eliminar (delete)</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
-    <t>denegar-actualizar/eliminar</t>
-  </si>
-  <si>
-    <t>modificar/tratada</t>
-  </si>
-  <si>
     <t>score</t>
   </si>
   <si>
-    <t>eliminar</t>
-  </si>
-  <si>
-    <t>modificar</t>
-  </si>
-  <si>
     <t>comunidades</t>
   </si>
   <si>
@@ -234,27 +208,15 @@
     <t>state</t>
   </si>
   <si>
-    <t>Actualizar(usuario)</t>
-  </si>
-  <si>
     <t>surname</t>
   </si>
   <si>
     <t>price</t>
   </si>
   <si>
-    <t>eliminar(delete)</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
-    <t>listar</t>
-  </si>
-  <si>
-    <t>delete</t>
-  </si>
-  <si>
     <t>capital_id</t>
   </si>
   <si>
@@ -270,21 +232,9 @@
     <t>rooms</t>
   </si>
   <si>
-    <t>Leer(uuid)</t>
-  </si>
-  <si>
     <t>content</t>
   </si>
   <si>
-    <t xml:space="preserve">actualizar </t>
-  </si>
-  <si>
-    <t>consultar</t>
-  </si>
-  <si>
-    <t>reportar</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -294,27 +244,15 @@
     <t>report_id</t>
   </si>
   <si>
-    <t>Eliminar(admin)</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
-    <t>leer</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
-    <t>Marcar eliminado</t>
-  </si>
-  <si>
     <t>bath</t>
   </si>
   <si>
-    <t>denunciar</t>
-  </si>
-  <si>
     <t>1 Bloqueada</t>
   </si>
   <si>
@@ -333,12 +271,6 @@
     <t>localidad_id</t>
   </si>
   <si>
-    <t>Identificarse</t>
-  </si>
-  <si>
-    <t>comentar</t>
-  </si>
-  <si>
     <t>3 Aceptada</t>
   </si>
   <si>
@@ -348,21 +280,12 @@
     <t>ciudad_id</t>
   </si>
   <si>
-    <t>Registrarse</t>
-  </si>
-  <si>
-    <t>valorar</t>
-  </si>
-  <si>
     <t>4 Descartada</t>
   </si>
   <si>
     <t>provincia_id</t>
   </si>
   <si>
-    <t>Logout</t>
-  </si>
-  <si>
     <t>0 Neutro</t>
   </si>
   <si>
@@ -372,9 +295,6 @@
     <t>pet_aceptada</t>
   </si>
   <si>
-    <t>listar(provincias)</t>
-  </si>
-  <si>
     <t>activar cuenta</t>
   </si>
   <si>
@@ -385,29 +305,200 @@
   </si>
   <si>
     <t>Guest</t>
+  </si>
+  <si>
+    <t>Iniciar Sesión</t>
+  </si>
+  <si>
+    <t>Cerrar Sesión</t>
+  </si>
+  <si>
+    <t>Consultar Usuario</t>
+  </si>
+  <si>
+    <t>Modificar Usuario</t>
+  </si>
+  <si>
+    <t>Eliminar Usuario</t>
+  </si>
+  <si>
+    <t>Reportar Usuario</t>
+  </si>
+  <si>
+    <t>Crear Usuario</t>
+  </si>
+  <si>
+    <t>Listar Usuarios</t>
+  </si>
+  <si>
+    <t>Bloquear Usuario</t>
+  </si>
+  <si>
+    <t>Desbloquear Usuario</t>
+  </si>
+  <si>
+    <t>Registrar Usuario</t>
+  </si>
+  <si>
+    <t>Creaer Anuncio</t>
+  </si>
+  <si>
+    <t>Consultar Anuncio</t>
+  </si>
+  <si>
+    <t>Listar Anuncios</t>
+  </si>
+  <si>
+    <t>Modificar Anuncio</t>
+  </si>
+  <si>
+    <t>Eliminar Anuncio</t>
+  </si>
+  <si>
+    <t>Comentar Anuncio</t>
+  </si>
+  <si>
+    <t>Valorar Anuncio</t>
+  </si>
+  <si>
+    <t>Denunciar Anuncio</t>
+  </si>
+  <si>
+    <t>Consultar Petición</t>
+  </si>
+  <si>
+    <t>Aceptar Petición</t>
+  </si>
+  <si>
+    <t>Denunciar Petición</t>
+  </si>
+  <si>
+    <t>Listar Peticiones</t>
+  </si>
+  <si>
+    <t>Descartar Petición</t>
+  </si>
+  <si>
+    <t>Eliminar Petición</t>
+  </si>
+  <si>
+    <t>Crear Petición</t>
+  </si>
+  <si>
+    <t>Denuncias</t>
+  </si>
+  <si>
+    <t>Listar Denuncias</t>
+  </si>
+  <si>
+    <t>Consultar Denuncia</t>
+  </si>
+  <si>
+    <t>Aceptar Denuncia</t>
+  </si>
+  <si>
+    <t>Rechazar Denuncia</t>
+  </si>
+  <si>
+    <t>Listar Comentarios</t>
+  </si>
+  <si>
+    <t>Denunciar Comentario</t>
+  </si>
+  <si>
+    <t>Eliminar Comentario</t>
+  </si>
+  <si>
+    <t>Valorar</t>
+  </si>
+  <si>
+    <t>Crear Tipo Vivienda</t>
+  </si>
+  <si>
+    <t>Listar Tipos Vivienda</t>
+  </si>
+  <si>
+    <t>Crear Tipo Operación</t>
+  </si>
+  <si>
+    <t>Listar Tipos Operación</t>
+  </si>
+  <si>
+    <t>Modificar Tipo Vivienda</t>
+  </si>
+  <si>
+    <t>Eliminar Tipo Vivienda</t>
+  </si>
+  <si>
+    <t>Modificar Tipo Operación</t>
+  </si>
+  <si>
+    <t>Eliminar Tipo Operación</t>
+  </si>
+  <si>
+    <t>Entidad</t>
+  </si>
+  <si>
+    <t>CREAR</t>
+  </si>
+  <si>
+    <t>ACTUALIZAR</t>
+  </si>
+  <si>
+    <t>CONSULTAR</t>
+  </si>
+  <si>
+    <t>BORRAR</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -421,9 +512,33 @@
         <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -437,77 +552,404 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF00CC00"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.14"/>
-    <col customWidth="1" min="3" max="3" width="23.29"/>
-    <col customWidth="1" min="4" max="4" width="19.29"/>
-    <col customWidth="1" min="6" max="6" width="22.43"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -518,149 +960,153 @@
         <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2">
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>56</v>
+        <v>125</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3">
+        <v>131</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="4" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="4" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>79</v>
+        <v>135</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="E5" s="14"/>
       <c r="F5" s="6"/>
       <c r="G5" s="4" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -671,15 +1117,15 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -690,14 +1136,16 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>111</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>118</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -707,12 +1155,12 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
@@ -724,13 +1172,11 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>112</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B10" s="14"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -741,81 +1187,82 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>103</v>
+      </c>
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -823,7 +1270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -831,7 +1278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -839,7 +1286,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -847,7 +1294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -855,17 +1302,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -873,12 +1320,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -886,7 +1333,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -894,294 +1341,297 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="6" max="6" width="19.14"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="B3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="L3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="G4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="K4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="5" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="M5" s="5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="5" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="6"/>
@@ -1192,15 +1642,15 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D8" s="6"/>
       <c r="F8" s="6"/>
@@ -1211,18 +1661,18 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1234,15 +1684,15 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -1255,15 +1705,15 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1276,15 +1726,15 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -1297,12 +1747,12 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1316,10 +1766,10 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1333,10 +1783,10 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="5" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1350,10 +1800,10 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1367,10 +1817,10 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="5" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1384,7 +1834,7 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -1399,6 +1849,232 @@
       <c r="M18" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511520A7-B11B-4F30-AB1A-83EB695DC5B6}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="E14" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
añadido manual de usuario GUEST completo y casi todo de usuario registrado
</commit_message>
<xml_diff>
--- a/PA_Proyecto.xlsx
+++ b/PA_Proyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\CorePHPMVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22231EE3-AA03-4852-BCB3-200D6170EAF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E06E5C2-9D6B-4C43-BE3D-F00DDED4F4DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="144">
   <si>
     <t>TODO</t>
   </si>
@@ -340,9 +340,6 @@
     <t>Registrar Usuario</t>
   </si>
   <si>
-    <t>Creaer Anuncio</t>
-  </si>
-  <si>
     <t>Consultar Anuncio</t>
   </si>
   <si>
@@ -452,6 +449,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Crear Anuncio</t>
+  </si>
+  <si>
+    <t>Desbloquear Anuncio</t>
   </si>
 </sst>
 </file>
@@ -935,13 +938,14 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
@@ -960,7 +964,7 @@
         <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>33</v>
@@ -989,25 +993,25 @@
         <v>94</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>129</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>78</v>
@@ -1024,23 +1028,23 @@
         <v>95</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -1051,23 +1055,23 @@
         <v>96</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -1078,21 +1082,21 @@
         <v>97</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="6"/>
       <c r="G5" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -1103,10 +1107,10 @@
         <v>98</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1122,10 +1126,10 @@
         <v>99</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1141,10 +1145,10 @@
         <v>100</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1160,7 +1164,7 @@
         <v>101</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
@@ -1176,7 +1180,9 @@
       <c r="A10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="14"/>
+      <c r="B10" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1235,8 +1241,8 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1857,7 +1863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511520A7-B11B-4F30-AB1A-83EB695DC5B6}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
@@ -1869,19 +1875,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="17" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>140</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1889,16 +1895,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1906,16 +1912,16 @@
         <v>36</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1923,16 +1929,16 @@
         <v>38</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1940,13 +1946,13 @@
         <v>40</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E5" s="21"/>
     </row>
@@ -1955,14 +1961,14 @@
         <v>41</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -1970,13 +1976,13 @@
         <v>42</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E7" s="21"/>
     </row>
@@ -1985,16 +1991,16 @@
         <v>43</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2002,16 +2008,16 @@
         <v>44</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2021,7 +2027,7 @@
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10" s="21"/>
     </row>
@@ -2032,7 +2038,7 @@
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" s="21"/>
     </row>
@@ -2043,7 +2049,7 @@
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
       <c r="D12" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" s="21"/>
     </row>
@@ -2052,14 +2058,14 @@
         <v>48</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2069,7 +2075,7 @@
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" s="21"/>
     </row>

</xml_diff>